<commit_message>
Bug fix cost calculation / labour cost
</commit_message>
<xml_diff>
--- a/data/input/cost_data/PLA_cost_ind.xlsx
+++ b/data/input/cost_data/PLA_cost_ind.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikonagengast/Desktop/Paper_MA/Paper_Recycling_3/AHP_Monte_Carlo/data/cost/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikonagengast/Desktop/Paper_MA/Paper_Recycling_3/AHP_Monte_Carlo/data/input/cost_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFBEA1AF-E5B5-F34E-9484-993421E8D893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFEFDC5-8FE0-B448-90AC-54A435A4500E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11860" yWindow="4720" windowWidth="21740" windowHeight="16280" activeTab="3" xr2:uid="{9E23791E-A9D1-B24D-9D6E-42C1F180DBE7}"/>
+    <workbookView xWindow="16400" yWindow="500" windowWidth="17200" windowHeight="16280" activeTab="3" xr2:uid="{9E23791E-A9D1-B24D-9D6E-42C1F180DBE7}"/>
   </bookViews>
   <sheets>
     <sheet name="shredding" sheetId="1" r:id="rId1"/>
@@ -169,18 +169,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -498,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25CECAF4-10EE-7547-8F9A-E08E88E519F7}">
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -525,33 +524,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3" t="s">
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3" t="s">
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3" t="s">
+      <c r="M1" s="6"/>
+      <c r="N1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -620,7 +619,7 @@
       <c r="C3">
         <v>30</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>9.1360000000000003E-7</v>
       </c>
       <c r="E3">
@@ -632,7 +631,7 @@
       <c r="G3">
         <v>0.20699999999999999</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="4">
         <f>0.083*0.128</f>
         <v>1.0624000000000001E-2</v>
       </c>
@@ -685,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14329C3B-818D-974A-839B-1CDF92A21CC9}">
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="119" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView zoomScale="119" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -712,33 +711,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3" t="s">
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3" t="s">
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3" t="s">
+      <c r="M1" s="6"/>
+      <c r="N1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -820,7 +819,7 @@
       <c r="G3">
         <v>0.20699999999999999</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="4">
         <f>0.083*0.16</f>
         <v>1.328E-2</v>
       </c>
@@ -899,33 +898,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3" t="s">
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3" t="s">
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3" t="s">
+      <c r="M1" s="6"/>
+      <c r="N1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -1055,8 +1054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C261B8B2-5703-4A47-9A2B-A87AD92FEE9B}">
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="143" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="143" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1082,34 +1081,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3" t="s">
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3" t="s">
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3" t="s">
+      <c r="M1" s="6"/>
+      <c r="N1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -1178,11 +1177,11 @@
       <c r="C3" s="2">
         <v>50</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="3">
         <v>2.385E-5</v>
       </c>
-      <c r="E3" s="7">
-        <v>35.1</v>
+      <c r="E3" s="5">
+        <v>0.20399999999999999</v>
       </c>
       <c r="F3" s="1">
         <v>1</v>
@@ -1196,7 +1195,7 @@
       <c r="I3">
         <v>0</v>
       </c>
-      <c r="J3" s="7">
+      <c r="J3" s="5">
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="K3">

</xml_diff>